<commit_message>
New functionalities added, HS added
</commit_message>
<xml_diff>
--- a/Comp and Socio Syllabus.xlsx
+++ b/Comp and Socio Syllabus.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\aditya data\Freelance Projects\Automation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F7E2767-112E-4DDE-804D-DEAE503F3E85}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF1D836D-1D0B-4EAA-BC92-930F44EA6CEF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -8544,6 +8544,50 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -8562,50 +8606,6 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -18663,169 +18663,169 @@
       <c r="X2" s="5"/>
       <c r="Y2" s="5"/>
       <c r="Z2" s="12"/>
-      <c r="AA2" s="43" t="s">
+      <c r="AA2" s="32" t="s">
         <v>1626</v>
       </c>
-      <c r="AB2" s="44"/>
-      <c r="AC2" s="44"/>
-      <c r="AD2" s="44"/>
-      <c r="AE2" s="44"/>
-      <c r="AF2" s="44"/>
-      <c r="AG2" s="44"/>
-      <c r="AH2" s="44"/>
-      <c r="AI2" s="44"/>
-      <c r="AJ2" s="44"/>
-      <c r="AK2" s="44"/>
-      <c r="AL2" s="44"/>
-      <c r="AM2" s="44"/>
-      <c r="AN2" s="44"/>
-      <c r="AO2" s="44"/>
-      <c r="AP2" s="44"/>
-      <c r="AQ2" s="44"/>
-      <c r="AR2" s="45"/>
-      <c r="AS2" s="43" t="s">
+      <c r="AB2" s="33"/>
+      <c r="AC2" s="33"/>
+      <c r="AD2" s="33"/>
+      <c r="AE2" s="33"/>
+      <c r="AF2" s="33"/>
+      <c r="AG2" s="33"/>
+      <c r="AH2" s="33"/>
+      <c r="AI2" s="33"/>
+      <c r="AJ2" s="33"/>
+      <c r="AK2" s="33"/>
+      <c r="AL2" s="33"/>
+      <c r="AM2" s="33"/>
+      <c r="AN2" s="33"/>
+      <c r="AO2" s="33"/>
+      <c r="AP2" s="33"/>
+      <c r="AQ2" s="33"/>
+      <c r="AR2" s="34"/>
+      <c r="AS2" s="32" t="s">
         <v>1627</v>
       </c>
-      <c r="AT2" s="44"/>
-      <c r="AU2" s="44"/>
-      <c r="AV2" s="44"/>
-      <c r="AW2" s="44"/>
-      <c r="AX2" s="44"/>
-      <c r="AY2" s="44"/>
-      <c r="AZ2" s="44"/>
-      <c r="BA2" s="44"/>
-      <c r="BB2" s="44"/>
-      <c r="BC2" s="44"/>
-      <c r="BD2" s="44"/>
-      <c r="BE2" s="44"/>
-      <c r="BF2" s="44"/>
-      <c r="BG2" s="44"/>
-      <c r="BH2" s="44"/>
-      <c r="BI2" s="44"/>
-      <c r="BJ2" s="44"/>
-      <c r="BK2" s="44"/>
-      <c r="BL2" s="44"/>
-      <c r="BM2" s="44"/>
-      <c r="BN2" s="44"/>
-      <c r="BO2" s="44"/>
-      <c r="BP2" s="45"/>
-      <c r="BQ2" s="32" t="s">
+      <c r="AT2" s="33"/>
+      <c r="AU2" s="33"/>
+      <c r="AV2" s="33"/>
+      <c r="AW2" s="33"/>
+      <c r="AX2" s="33"/>
+      <c r="AY2" s="33"/>
+      <c r="AZ2" s="33"/>
+      <c r="BA2" s="33"/>
+      <c r="BB2" s="33"/>
+      <c r="BC2" s="33"/>
+      <c r="BD2" s="33"/>
+      <c r="BE2" s="33"/>
+      <c r="BF2" s="33"/>
+      <c r="BG2" s="33"/>
+      <c r="BH2" s="33"/>
+      <c r="BI2" s="33"/>
+      <c r="BJ2" s="33"/>
+      <c r="BK2" s="33"/>
+      <c r="BL2" s="33"/>
+      <c r="BM2" s="33"/>
+      <c r="BN2" s="33"/>
+      <c r="BO2" s="33"/>
+      <c r="BP2" s="34"/>
+      <c r="BQ2" s="29" t="s">
         <v>1628</v>
       </c>
-      <c r="BR2" s="46"/>
-      <c r="BS2" s="46"/>
-      <c r="BT2" s="46"/>
-      <c r="BU2" s="46"/>
-      <c r="BV2" s="46"/>
-      <c r="BW2" s="46"/>
-      <c r="BX2" s="46"/>
-      <c r="BY2" s="46"/>
-      <c r="BZ2" s="46"/>
-      <c r="CA2" s="46"/>
-      <c r="CB2" s="47"/>
-      <c r="CC2" s="43" t="s">
+      <c r="BR2" s="35"/>
+      <c r="BS2" s="35"/>
+      <c r="BT2" s="35"/>
+      <c r="BU2" s="35"/>
+      <c r="BV2" s="35"/>
+      <c r="BW2" s="35"/>
+      <c r="BX2" s="35"/>
+      <c r="BY2" s="35"/>
+      <c r="BZ2" s="35"/>
+      <c r="CA2" s="35"/>
+      <c r="CB2" s="36"/>
+      <c r="CC2" s="32" t="s">
         <v>1629</v>
       </c>
-      <c r="CD2" s="44"/>
-      <c r="CE2" s="44"/>
-      <c r="CF2" s="44"/>
-      <c r="CG2" s="44"/>
-      <c r="CH2" s="44"/>
-      <c r="CI2" s="44"/>
-      <c r="CJ2" s="44"/>
-      <c r="CK2" s="44"/>
-      <c r="CL2" s="44"/>
-      <c r="CM2" s="44"/>
-      <c r="CN2" s="44"/>
-      <c r="CO2" s="44"/>
-      <c r="CP2" s="44"/>
-      <c r="CQ2" s="44"/>
-      <c r="CR2" s="45"/>
-      <c r="CS2" s="40" t="s">
+      <c r="CD2" s="33"/>
+      <c r="CE2" s="33"/>
+      <c r="CF2" s="33"/>
+      <c r="CG2" s="33"/>
+      <c r="CH2" s="33"/>
+      <c r="CI2" s="33"/>
+      <c r="CJ2" s="33"/>
+      <c r="CK2" s="33"/>
+      <c r="CL2" s="33"/>
+      <c r="CM2" s="33"/>
+      <c r="CN2" s="33"/>
+      <c r="CO2" s="33"/>
+      <c r="CP2" s="33"/>
+      <c r="CQ2" s="33"/>
+      <c r="CR2" s="34"/>
+      <c r="CS2" s="26" t="s">
         <v>1630</v>
       </c>
-      <c r="CT2" s="41"/>
-      <c r="CU2" s="41"/>
-      <c r="CV2" s="41"/>
-      <c r="CW2" s="41"/>
-      <c r="CX2" s="41"/>
-      <c r="CY2" s="41"/>
-      <c r="CZ2" s="41"/>
-      <c r="DA2" s="41"/>
-      <c r="DB2" s="41"/>
-      <c r="DC2" s="41"/>
-      <c r="DD2" s="41"/>
-      <c r="DE2" s="41"/>
-      <c r="DF2" s="42"/>
-      <c r="DG2" s="40" t="s">
+      <c r="CT2" s="27"/>
+      <c r="CU2" s="27"/>
+      <c r="CV2" s="27"/>
+      <c r="CW2" s="27"/>
+      <c r="CX2" s="27"/>
+      <c r="CY2" s="27"/>
+      <c r="CZ2" s="27"/>
+      <c r="DA2" s="27"/>
+      <c r="DB2" s="27"/>
+      <c r="DC2" s="27"/>
+      <c r="DD2" s="27"/>
+      <c r="DE2" s="27"/>
+      <c r="DF2" s="28"/>
+      <c r="DG2" s="26" t="s">
         <v>1631</v>
       </c>
-      <c r="DH2" s="41"/>
-      <c r="DI2" s="41"/>
-      <c r="DJ2" s="41"/>
-      <c r="DK2" s="41"/>
-      <c r="DL2" s="41"/>
-      <c r="DM2" s="41"/>
-      <c r="DN2" s="41"/>
-      <c r="DO2" s="41"/>
-      <c r="DP2" s="41"/>
-      <c r="DQ2" s="41"/>
-      <c r="DR2" s="42"/>
-      <c r="DS2" s="40" t="s">
+      <c r="DH2" s="27"/>
+      <c r="DI2" s="27"/>
+      <c r="DJ2" s="27"/>
+      <c r="DK2" s="27"/>
+      <c r="DL2" s="27"/>
+      <c r="DM2" s="27"/>
+      <c r="DN2" s="27"/>
+      <c r="DO2" s="27"/>
+      <c r="DP2" s="27"/>
+      <c r="DQ2" s="27"/>
+      <c r="DR2" s="28"/>
+      <c r="DS2" s="26" t="s">
         <v>1632</v>
       </c>
-      <c r="DT2" s="41"/>
-      <c r="DU2" s="41"/>
-      <c r="DV2" s="41"/>
-      <c r="DW2" s="41"/>
-      <c r="DX2" s="41"/>
-      <c r="DY2" s="41"/>
-      <c r="DZ2" s="41"/>
-      <c r="EA2" s="41"/>
-      <c r="EB2" s="41"/>
-      <c r="EC2" s="41"/>
-      <c r="ED2" s="42"/>
-      <c r="EE2" s="40" t="s">
+      <c r="DT2" s="27"/>
+      <c r="DU2" s="27"/>
+      <c r="DV2" s="27"/>
+      <c r="DW2" s="27"/>
+      <c r="DX2" s="27"/>
+      <c r="DY2" s="27"/>
+      <c r="DZ2" s="27"/>
+      <c r="EA2" s="27"/>
+      <c r="EB2" s="27"/>
+      <c r="EC2" s="27"/>
+      <c r="ED2" s="28"/>
+      <c r="EE2" s="26" t="s">
         <v>1633</v>
       </c>
-      <c r="EF2" s="41"/>
-      <c r="EG2" s="41"/>
-      <c r="EH2" s="41"/>
-      <c r="EI2" s="41"/>
-      <c r="EJ2" s="41"/>
-      <c r="EK2" s="41"/>
-      <c r="EL2" s="41"/>
-      <c r="EM2" s="41"/>
-      <c r="EN2" s="41"/>
-      <c r="EO2" s="41"/>
-      <c r="EP2" s="42"/>
-      <c r="EQ2" s="40" t="s">
+      <c r="EF2" s="27"/>
+      <c r="EG2" s="27"/>
+      <c r="EH2" s="27"/>
+      <c r="EI2" s="27"/>
+      <c r="EJ2" s="27"/>
+      <c r="EK2" s="27"/>
+      <c r="EL2" s="27"/>
+      <c r="EM2" s="27"/>
+      <c r="EN2" s="27"/>
+      <c r="EO2" s="27"/>
+      <c r="EP2" s="28"/>
+      <c r="EQ2" s="26" t="s">
         <v>1634</v>
       </c>
-      <c r="ER2" s="41"/>
-      <c r="ES2" s="41"/>
-      <c r="ET2" s="41"/>
-      <c r="EU2" s="41"/>
-      <c r="EV2" s="41"/>
-      <c r="EW2" s="41"/>
-      <c r="EX2" s="41"/>
-      <c r="EY2" s="41"/>
-      <c r="EZ2" s="41"/>
-      <c r="FA2" s="41"/>
-      <c r="FB2" s="41"/>
-      <c r="FC2" s="41"/>
-      <c r="FD2" s="41"/>
-      <c r="FE2" s="41"/>
-      <c r="FF2" s="41"/>
-      <c r="FG2" s="41"/>
-      <c r="FH2" s="42"/>
+      <c r="ER2" s="27"/>
+      <c r="ES2" s="27"/>
+      <c r="ET2" s="27"/>
+      <c r="EU2" s="27"/>
+      <c r="EV2" s="27"/>
+      <c r="EW2" s="27"/>
+      <c r="EX2" s="27"/>
+      <c r="EY2" s="27"/>
+      <c r="EZ2" s="27"/>
+      <c r="FA2" s="27"/>
+      <c r="FB2" s="27"/>
+      <c r="FC2" s="27"/>
+      <c r="FD2" s="27"/>
+      <c r="FE2" s="27"/>
+      <c r="FF2" s="27"/>
+      <c r="FG2" s="27"/>
+      <c r="FH2" s="28"/>
     </row>
     <row r="3" spans="1:164" ht="30.75" customHeight="1">
-      <c r="A3" s="32" t="s">
+      <c r="A3" s="29" t="s">
         <v>1635</v>
       </c>
-      <c r="B3" s="33"/>
-      <c r="C3" s="39"/>
+      <c r="B3" s="30"/>
+      <c r="C3" s="31"/>
     </row>
     <row r="4" spans="1:164" ht="28.2">
       <c r="A4" s="6" t="s">
@@ -18839,13 +18839,13 @@
       </c>
     </row>
     <row r="5" spans="1:164">
-      <c r="A5" s="32" t="s">
+      <c r="A5" s="29" t="s">
         <v>1639</v>
       </c>
-      <c r="B5" s="33"/>
-      <c r="C5" s="33"/>
-      <c r="D5" s="33"/>
-      <c r="E5" s="39"/>
+      <c r="B5" s="30"/>
+      <c r="C5" s="30"/>
+      <c r="D5" s="30"/>
+      <c r="E5" s="31"/>
     </row>
     <row r="6" spans="1:164" ht="42">
       <c r="A6" s="6" t="s">
@@ -18865,14 +18865,14 @@
       </c>
     </row>
     <row r="7" spans="1:164">
-      <c r="A7" s="32" t="s">
+      <c r="A7" s="29" t="s">
         <v>1645</v>
       </c>
-      <c r="B7" s="33"/>
-      <c r="C7" s="33"/>
-      <c r="D7" s="33"/>
-      <c r="E7" s="33"/>
-      <c r="F7" s="39"/>
+      <c r="B7" s="30"/>
+      <c r="C7" s="30"/>
+      <c r="D7" s="30"/>
+      <c r="E7" s="30"/>
+      <c r="F7" s="31"/>
     </row>
     <row r="8" spans="1:164" ht="28.2">
       <c r="A8" s="6" t="s">
@@ -18895,14 +18895,14 @@
       </c>
     </row>
     <row r="9" spans="1:164">
-      <c r="A9" s="32" t="s">
+      <c r="A9" s="29" t="s">
         <v>1652</v>
       </c>
-      <c r="B9" s="33"/>
-      <c r="C9" s="33"/>
-      <c r="D9" s="33"/>
-      <c r="E9" s="33"/>
-      <c r="F9" s="39"/>
+      <c r="B9" s="30"/>
+      <c r="C9" s="30"/>
+      <c r="D9" s="30"/>
+      <c r="E9" s="30"/>
+      <c r="F9" s="31"/>
     </row>
     <row r="10" spans="1:164" ht="28.2">
       <c r="A10" s="6" t="s">
@@ -18925,14 +18925,14 @@
       </c>
     </row>
     <row r="11" spans="1:164">
-      <c r="A11" s="32" t="s">
+      <c r="A11" s="29" t="s">
         <v>1659</v>
       </c>
-      <c r="B11" s="33"/>
-      <c r="C11" s="33"/>
-      <c r="D11" s="33"/>
-      <c r="E11" s="33"/>
-      <c r="F11" s="39"/>
+      <c r="B11" s="30"/>
+      <c r="C11" s="30"/>
+      <c r="D11" s="30"/>
+      <c r="E11" s="30"/>
+      <c r="F11" s="31"/>
     </row>
     <row r="12" spans="1:164" ht="55.8">
       <c r="A12" s="6" t="s">
@@ -18955,13 +18955,13 @@
       </c>
     </row>
     <row r="13" spans="1:164">
-      <c r="A13" s="32" t="s">
+      <c r="A13" s="29" t="s">
         <v>1666</v>
       </c>
-      <c r="B13" s="33"/>
-      <c r="C13" s="33"/>
-      <c r="D13" s="33"/>
-      <c r="E13" s="39"/>
+      <c r="B13" s="30"/>
+      <c r="C13" s="30"/>
+      <c r="D13" s="30"/>
+      <c r="E13" s="31"/>
     </row>
     <row r="14" spans="1:164" ht="97.2">
       <c r="A14" s="6" t="s">
@@ -18981,12 +18981,12 @@
       </c>
     </row>
     <row r="15" spans="1:164">
-      <c r="A15" s="32" t="s">
+      <c r="A15" s="29" t="s">
         <v>1672</v>
       </c>
-      <c r="B15" s="33"/>
-      <c r="C15" s="33"/>
-      <c r="D15" s="39"/>
+      <c r="B15" s="30"/>
+      <c r="C15" s="30"/>
+      <c r="D15" s="31"/>
     </row>
     <row r="16" spans="1:164" ht="55.8">
       <c r="A16" s="6" t="s">
@@ -19003,12 +19003,12 @@
       </c>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="32" t="s">
+      <c r="A17" s="29" t="s">
         <v>1677</v>
       </c>
-      <c r="B17" s="33"/>
-      <c r="C17" s="33"/>
-      <c r="D17" s="39"/>
+      <c r="B17" s="30"/>
+      <c r="C17" s="30"/>
+      <c r="D17" s="31"/>
     </row>
     <row r="18" spans="1:10" ht="28.2">
       <c r="A18" s="6" t="s">
@@ -19025,13 +19025,13 @@
       </c>
     </row>
     <row r="19" spans="1:10">
-      <c r="A19" s="32" t="s">
+      <c r="A19" s="29" t="s">
         <v>1682</v>
       </c>
-      <c r="B19" s="33"/>
-      <c r="C19" s="33"/>
-      <c r="D19" s="33"/>
-      <c r="E19" s="39"/>
+      <c r="B19" s="30"/>
+      <c r="C19" s="30"/>
+      <c r="D19" s="30"/>
+      <c r="E19" s="31"/>
     </row>
     <row r="20" spans="1:10" ht="42">
       <c r="A20" s="6" t="s">
@@ -19051,18 +19051,18 @@
       </c>
     </row>
     <row r="21" spans="1:10">
-      <c r="A21" s="32" t="s">
+      <c r="A21" s="29" t="s">
         <v>1688</v>
       </c>
-      <c r="B21" s="33"/>
-      <c r="C21" s="33"/>
-      <c r="D21" s="33"/>
-      <c r="E21" s="33"/>
-      <c r="F21" s="33"/>
-      <c r="G21" s="33"/>
-      <c r="H21" s="33"/>
-      <c r="I21" s="33"/>
-      <c r="J21" s="39"/>
+      <c r="B21" s="30"/>
+      <c r="C21" s="30"/>
+      <c r="D21" s="30"/>
+      <c r="E21" s="30"/>
+      <c r="F21" s="30"/>
+      <c r="G21" s="30"/>
+      <c r="H21" s="30"/>
+      <c r="I21" s="30"/>
+      <c r="J21" s="31"/>
     </row>
     <row r="22" spans="1:10" ht="69.599999999999994">
       <c r="A22" s="6" t="s">
@@ -19097,14 +19097,14 @@
       </c>
     </row>
     <row r="23" spans="1:10">
-      <c r="A23" s="32" t="s">
+      <c r="A23" s="29" t="s">
         <v>1699</v>
       </c>
-      <c r="B23" s="33"/>
-      <c r="C23" s="33"/>
-      <c r="D23" s="33"/>
-      <c r="E23" s="33"/>
-      <c r="F23" s="39"/>
+      <c r="B23" s="30"/>
+      <c r="C23" s="30"/>
+      <c r="D23" s="30"/>
+      <c r="E23" s="30"/>
+      <c r="F23" s="31"/>
     </row>
     <row r="24" spans="1:10" ht="28.2">
       <c r="A24" s="6" t="s">
@@ -19127,14 +19127,14 @@
       </c>
     </row>
     <row r="25" spans="1:10">
-      <c r="A25" s="32" t="s">
+      <c r="A25" s="29" t="s">
         <v>1706</v>
       </c>
-      <c r="B25" s="33"/>
-      <c r="C25" s="33"/>
-      <c r="D25" s="39"/>
-    </row>
-    <row r="26" spans="1:10" ht="69.599999999999994">
+      <c r="B25" s="30"/>
+      <c r="C25" s="30"/>
+      <c r="D25" s="31"/>
+    </row>
+    <row r="26" spans="1:10" ht="55.8">
       <c r="A26" s="6" t="s">
         <v>1707</v>
       </c>
@@ -19149,12 +19149,12 @@
       </c>
     </row>
     <row r="27" spans="1:10">
-      <c r="A27" s="32" t="s">
+      <c r="A27" s="29" t="s">
         <v>1711</v>
       </c>
-      <c r="B27" s="33"/>
-      <c r="C27" s="33"/>
-      <c r="D27" s="39"/>
+      <c r="B27" s="30"/>
+      <c r="C27" s="30"/>
+      <c r="D27" s="31"/>
     </row>
     <row r="28" spans="1:10" ht="83.4">
       <c r="A28" s="6" t="s">
@@ -19171,14 +19171,14 @@
       </c>
     </row>
     <row r="29" spans="1:10">
-      <c r="A29" s="32" t="s">
+      <c r="A29" s="29" t="s">
         <v>1716</v>
       </c>
-      <c r="B29" s="33"/>
-      <c r="C29" s="33"/>
-      <c r="D29" s="33"/>
-      <c r="E29" s="33"/>
-      <c r="F29" s="39"/>
+      <c r="B29" s="30"/>
+      <c r="C29" s="30"/>
+      <c r="D29" s="30"/>
+      <c r="E29" s="30"/>
+      <c r="F29" s="31"/>
     </row>
     <row r="30" spans="1:10" ht="97.2">
       <c r="A30" s="9" t="s">
@@ -19201,14 +19201,14 @@
       </c>
     </row>
     <row r="31" spans="1:10">
-      <c r="A31" s="32" t="s">
+      <c r="A31" s="29" t="s">
         <v>1723</v>
       </c>
-      <c r="B31" s="33"/>
-      <c r="C31" s="33"/>
-      <c r="D31" s="33"/>
-      <c r="E31" s="33"/>
-      <c r="F31" s="39"/>
+      <c r="B31" s="30"/>
+      <c r="C31" s="30"/>
+      <c r="D31" s="30"/>
+      <c r="E31" s="30"/>
+      <c r="F31" s="31"/>
     </row>
     <row r="32" spans="1:10" ht="69.599999999999994">
       <c r="A32" s="9" t="s">
@@ -19231,18 +19231,18 @@
       </c>
     </row>
     <row r="33" spans="1:68">
-      <c r="A33" s="32" t="s">
+      <c r="A33" s="29" t="s">
         <v>1730</v>
       </c>
-      <c r="B33" s="33"/>
-      <c r="C33" s="33"/>
-      <c r="D33" s="33"/>
-      <c r="E33" s="33"/>
-      <c r="F33" s="33"/>
-      <c r="G33" s="33"/>
-      <c r="H33" s="33"/>
-      <c r="I33" s="33"/>
-      <c r="J33" s="39"/>
+      <c r="B33" s="30"/>
+      <c r="C33" s="30"/>
+      <c r="D33" s="30"/>
+      <c r="E33" s="30"/>
+      <c r="F33" s="30"/>
+      <c r="G33" s="30"/>
+      <c r="H33" s="30"/>
+      <c r="I33" s="30"/>
+      <c r="J33" s="31"/>
     </row>
     <row r="34" spans="1:68" ht="83.4">
       <c r="A34" s="6" t="s">
@@ -19277,14 +19277,14 @@
       </c>
     </row>
     <row r="35" spans="1:68">
-      <c r="A35" s="32" t="s">
+      <c r="A35" s="29" t="s">
         <v>1741</v>
       </c>
-      <c r="B35" s="33"/>
-      <c r="C35" s="33"/>
-      <c r="D35" s="33"/>
-      <c r="E35" s="33"/>
-      <c r="F35" s="34"/>
+      <c r="B35" s="30"/>
+      <c r="C35" s="30"/>
+      <c r="D35" s="30"/>
+      <c r="E35" s="30"/>
+      <c r="F35" s="37"/>
     </row>
     <row r="36" spans="1:68" ht="111">
       <c r="A36" s="6" t="s">
@@ -19307,284 +19307,368 @@
       </c>
     </row>
     <row r="37" spans="1:68">
-      <c r="A37" s="35" t="s">
+      <c r="A37" s="38" t="s">
         <v>1748</v>
       </c>
-      <c r="B37" s="37" t="s">
+      <c r="B37" s="40" t="s">
         <v>1749</v>
       </c>
-      <c r="C37" s="37" t="s">
+      <c r="C37" s="40" t="s">
         <v>1750</v>
       </c>
-      <c r="D37" s="37" t="s">
+      <c r="D37" s="40" t="s">
         <v>1751</v>
       </c>
-      <c r="E37" s="37" t="s">
+      <c r="E37" s="40" t="s">
         <v>1752</v>
       </c>
-      <c r="F37" s="37" t="s">
+      <c r="F37" s="40" t="s">
         <v>1753</v>
       </c>
-      <c r="G37" s="26" t="s">
+      <c r="G37" s="42" t="s">
         <v>1754</v>
       </c>
-      <c r="H37" s="26" t="s">
+      <c r="H37" s="42" t="s">
         <v>1755</v>
       </c>
-      <c r="I37" s="26" t="s">
+      <c r="I37" s="42" t="s">
         <v>1756</v>
       </c>
-      <c r="J37" s="26" t="s">
+      <c r="J37" s="42" t="s">
         <v>1757</v>
       </c>
-      <c r="K37" s="26" t="s">
+      <c r="K37" s="42" t="s">
         <v>1758</v>
       </c>
-      <c r="L37" s="26" t="s">
+      <c r="L37" s="42" t="s">
         <v>1759</v>
       </c>
-      <c r="M37" s="26" t="s">
+      <c r="M37" s="42" t="s">
         <v>1760</v>
       </c>
-      <c r="N37" s="28" t="s">
+      <c r="N37" s="44" t="s">
         <v>1761</v>
       </c>
-      <c r="O37" s="30" t="s">
+      <c r="O37" s="46" t="s">
         <v>1762</v>
       </c>
-      <c r="P37" s="26" t="s">
+      <c r="P37" s="42" t="s">
         <v>1763</v>
       </c>
-      <c r="Q37" s="26" t="s">
+      <c r="Q37" s="42" t="s">
         <v>1764</v>
       </c>
-      <c r="R37" s="26" t="s">
+      <c r="R37" s="42" t="s">
         <v>1765</v>
       </c>
-      <c r="S37" s="26" t="s">
+      <c r="S37" s="42" t="s">
         <v>1766</v>
       </c>
-      <c r="T37" s="26" t="s">
+      <c r="T37" s="42" t="s">
         <v>1767</v>
       </c>
-      <c r="U37" s="26" t="s">
+      <c r="U37" s="42" t="s">
         <v>1768</v>
       </c>
-      <c r="V37" s="26" t="s">
+      <c r="V37" s="42" t="s">
         <v>1769</v>
       </c>
-      <c r="W37" s="26" t="s">
+      <c r="W37" s="42" t="s">
         <v>1770</v>
       </c>
-      <c r="X37" s="26" t="s">
+      <c r="X37" s="42" t="s">
         <v>1771</v>
       </c>
-      <c r="Y37" s="26" t="s">
+      <c r="Y37" s="42" t="s">
         <v>1772</v>
       </c>
-      <c r="Z37" s="28" t="s">
+      <c r="Z37" s="44" t="s">
         <v>1773</v>
       </c>
-      <c r="AA37" s="30" t="s">
+      <c r="AA37" s="46" t="s">
         <v>1774</v>
       </c>
-      <c r="AB37" s="26" t="s">
+      <c r="AB37" s="42" t="s">
         <v>1775</v>
       </c>
-      <c r="AC37" s="26" t="s">
+      <c r="AC37" s="42" t="s">
         <v>1776</v>
       </c>
-      <c r="AD37" s="26" t="s">
+      <c r="AD37" s="42" t="s">
         <v>1777</v>
       </c>
-      <c r="AE37" s="26" t="s">
+      <c r="AE37" s="42" t="s">
         <v>1778</v>
       </c>
-      <c r="AF37" s="26" t="s">
+      <c r="AF37" s="42" t="s">
         <v>1779</v>
       </c>
-      <c r="AG37" s="26" t="s">
+      <c r="AG37" s="42" t="s">
         <v>1780</v>
       </c>
-      <c r="AH37" s="26" t="s">
+      <c r="AH37" s="42" t="s">
         <v>1781</v>
       </c>
-      <c r="AI37" s="26" t="s">
+      <c r="AI37" s="42" t="s">
         <v>1782</v>
       </c>
-      <c r="AJ37" s="26" t="s">
+      <c r="AJ37" s="42" t="s">
         <v>1783</v>
       </c>
-      <c r="AK37" s="26" t="s">
+      <c r="AK37" s="42" t="s">
         <v>1784</v>
       </c>
-      <c r="AL37" s="28" t="s">
+      <c r="AL37" s="44" t="s">
         <v>1785</v>
       </c>
-      <c r="AM37" s="30" t="s">
+      <c r="AM37" s="46" t="s">
         <v>1786</v>
       </c>
-      <c r="AN37" s="26" t="s">
+      <c r="AN37" s="42" t="s">
         <v>1787</v>
       </c>
-      <c r="AO37" s="26" t="s">
+      <c r="AO37" s="42" t="s">
         <v>1788</v>
       </c>
-      <c r="AP37" s="26" t="s">
+      <c r="AP37" s="42" t="s">
         <v>1789</v>
       </c>
-      <c r="AQ37" s="26" t="s">
+      <c r="AQ37" s="42" t="s">
         <v>1790</v>
       </c>
-      <c r="AR37" s="26" t="s">
+      <c r="AR37" s="42" t="s">
         <v>1791</v>
       </c>
-      <c r="AS37" s="26" t="s">
+      <c r="AS37" s="42" t="s">
         <v>1792</v>
       </c>
-      <c r="AT37" s="26" t="s">
+      <c r="AT37" s="42" t="s">
         <v>1793</v>
       </c>
-      <c r="AU37" s="26" t="s">
+      <c r="AU37" s="42" t="s">
         <v>1794</v>
       </c>
-      <c r="AV37" s="26" t="s">
+      <c r="AV37" s="42" t="s">
         <v>1795</v>
       </c>
-      <c r="AW37" s="26" t="s">
+      <c r="AW37" s="42" t="s">
         <v>1796</v>
       </c>
-      <c r="AX37" s="28" t="s">
+      <c r="AX37" s="44" t="s">
         <v>1797</v>
       </c>
-      <c r="AY37" s="30" t="s">
+      <c r="AY37" s="46" t="s">
         <v>1798</v>
       </c>
-      <c r="AZ37" s="26" t="s">
+      <c r="AZ37" s="42" t="s">
         <v>1799</v>
       </c>
-      <c r="BA37" s="26" t="s">
+      <c r="BA37" s="42" t="s">
         <v>1800</v>
       </c>
-      <c r="BB37" s="26" t="s">
+      <c r="BB37" s="42" t="s">
         <v>1801</v>
       </c>
-      <c r="BC37" s="26" t="s">
+      <c r="BC37" s="42" t="s">
         <v>1802</v>
       </c>
-      <c r="BD37" s="26" t="s">
+      <c r="BD37" s="42" t="s">
         <v>1803</v>
       </c>
-      <c r="BE37" s="26" t="s">
+      <c r="BE37" s="42" t="s">
         <v>1804</v>
       </c>
-      <c r="BF37" s="26" t="s">
+      <c r="BF37" s="42" t="s">
         <v>1805</v>
       </c>
-      <c r="BG37" s="26" t="s">
+      <c r="BG37" s="42" t="s">
         <v>1806</v>
       </c>
-      <c r="BH37" s="26" t="s">
+      <c r="BH37" s="42" t="s">
         <v>1807</v>
       </c>
-      <c r="BI37" s="26" t="s">
+      <c r="BI37" s="42" t="s">
         <v>1808</v>
       </c>
-      <c r="BJ37" s="26" t="s">
+      <c r="BJ37" s="42" t="s">
         <v>1809</v>
       </c>
-      <c r="BK37" s="26" t="s">
+      <c r="BK37" s="42" t="s">
         <v>1810</v>
       </c>
-      <c r="BL37" s="26" t="s">
+      <c r="BL37" s="42" t="s">
         <v>1811</v>
       </c>
-      <c r="BM37" s="26" t="s">
+      <c r="BM37" s="42" t="s">
         <v>1812</v>
       </c>
-      <c r="BN37" s="26" t="s">
+      <c r="BN37" s="42" t="s">
         <v>1813</v>
       </c>
-      <c r="BO37" s="26" t="s">
+      <c r="BO37" s="42" t="s">
         <v>1814</v>
       </c>
-      <c r="BP37" s="28" t="s">
+      <c r="BP37" s="44" t="s">
         <v>1815</v>
       </c>
     </row>
     <row r="38" spans="1:68">
-      <c r="A38" s="36"/>
-      <c r="B38" s="38"/>
-      <c r="C38" s="38"/>
-      <c r="D38" s="38"/>
-      <c r="E38" s="38"/>
-      <c r="F38" s="38"/>
-      <c r="G38" s="27"/>
-      <c r="H38" s="27"/>
-      <c r="I38" s="27"/>
-      <c r="J38" s="27"/>
-      <c r="K38" s="27"/>
-      <c r="L38" s="27"/>
-      <c r="M38" s="27"/>
-      <c r="N38" s="29"/>
-      <c r="O38" s="31"/>
-      <c r="P38" s="27"/>
-      <c r="Q38" s="27"/>
-      <c r="R38" s="27"/>
-      <c r="S38" s="27"/>
-      <c r="T38" s="27"/>
-      <c r="U38" s="27"/>
-      <c r="V38" s="27"/>
-      <c r="W38" s="27"/>
-      <c r="X38" s="27"/>
-      <c r="Y38" s="27"/>
-      <c r="Z38" s="29"/>
-      <c r="AA38" s="31"/>
-      <c r="AB38" s="27"/>
-      <c r="AC38" s="27"/>
-      <c r="AD38" s="27"/>
-      <c r="AE38" s="27"/>
-      <c r="AF38" s="27"/>
-      <c r="AG38" s="27"/>
-      <c r="AH38" s="27"/>
-      <c r="AI38" s="27"/>
-      <c r="AJ38" s="27"/>
-      <c r="AK38" s="27"/>
-      <c r="AL38" s="29"/>
-      <c r="AM38" s="31"/>
-      <c r="AN38" s="27"/>
-      <c r="AO38" s="27"/>
-      <c r="AP38" s="27"/>
-      <c r="AQ38" s="27"/>
-      <c r="AR38" s="27"/>
-      <c r="AS38" s="27"/>
-      <c r="AT38" s="27"/>
-      <c r="AU38" s="27"/>
-      <c r="AV38" s="27"/>
-      <c r="AW38" s="27"/>
-      <c r="AX38" s="29"/>
-      <c r="AY38" s="31"/>
-      <c r="AZ38" s="27"/>
-      <c r="BA38" s="27"/>
-      <c r="BB38" s="27"/>
-      <c r="BC38" s="27"/>
-      <c r="BD38" s="27"/>
-      <c r="BE38" s="27"/>
-      <c r="BF38" s="27"/>
-      <c r="BG38" s="27"/>
-      <c r="BH38" s="27"/>
-      <c r="BI38" s="27"/>
-      <c r="BJ38" s="27"/>
-      <c r="BK38" s="27"/>
-      <c r="BL38" s="27"/>
-      <c r="BM38" s="27"/>
-      <c r="BN38" s="27"/>
-      <c r="BO38" s="27"/>
-      <c r="BP38" s="29"/>
+      <c r="A38" s="39"/>
+      <c r="B38" s="41"/>
+      <c r="C38" s="41"/>
+      <c r="D38" s="41"/>
+      <c r="E38" s="41"/>
+      <c r="F38" s="41"/>
+      <c r="G38" s="43"/>
+      <c r="H38" s="43"/>
+      <c r="I38" s="43"/>
+      <c r="J38" s="43"/>
+      <c r="K38" s="43"/>
+      <c r="L38" s="43"/>
+      <c r="M38" s="43"/>
+      <c r="N38" s="45"/>
+      <c r="O38" s="47"/>
+      <c r="P38" s="43"/>
+      <c r="Q38" s="43"/>
+      <c r="R38" s="43"/>
+      <c r="S38" s="43"/>
+      <c r="T38" s="43"/>
+      <c r="U38" s="43"/>
+      <c r="V38" s="43"/>
+      <c r="W38" s="43"/>
+      <c r="X38" s="43"/>
+      <c r="Y38" s="43"/>
+      <c r="Z38" s="45"/>
+      <c r="AA38" s="47"/>
+      <c r="AB38" s="43"/>
+      <c r="AC38" s="43"/>
+      <c r="AD38" s="43"/>
+      <c r="AE38" s="43"/>
+      <c r="AF38" s="43"/>
+      <c r="AG38" s="43"/>
+      <c r="AH38" s="43"/>
+      <c r="AI38" s="43"/>
+      <c r="AJ38" s="43"/>
+      <c r="AK38" s="43"/>
+      <c r="AL38" s="45"/>
+      <c r="AM38" s="47"/>
+      <c r="AN38" s="43"/>
+      <c r="AO38" s="43"/>
+      <c r="AP38" s="43"/>
+      <c r="AQ38" s="43"/>
+      <c r="AR38" s="43"/>
+      <c r="AS38" s="43"/>
+      <c r="AT38" s="43"/>
+      <c r="AU38" s="43"/>
+      <c r="AV38" s="43"/>
+      <c r="AW38" s="43"/>
+      <c r="AX38" s="45"/>
+      <c r="AY38" s="47"/>
+      <c r="AZ38" s="43"/>
+      <c r="BA38" s="43"/>
+      <c r="BB38" s="43"/>
+      <c r="BC38" s="43"/>
+      <c r="BD38" s="43"/>
+      <c r="BE38" s="43"/>
+      <c r="BF38" s="43"/>
+      <c r="BG38" s="43"/>
+      <c r="BH38" s="43"/>
+      <c r="BI38" s="43"/>
+      <c r="BJ38" s="43"/>
+      <c r="BK38" s="43"/>
+      <c r="BL38" s="43"/>
+      <c r="BM38" s="43"/>
+      <c r="BN38" s="43"/>
+      <c r="BO38" s="43"/>
+      <c r="BP38" s="45"/>
     </row>
     <row r="123" ht="15" customHeight="1"/>
   </sheetData>
   <mergeCells count="94">
+    <mergeCell ref="BO37:BO38"/>
+    <mergeCell ref="BP37:BP38"/>
+    <mergeCell ref="BJ37:BJ38"/>
+    <mergeCell ref="BK37:BK38"/>
+    <mergeCell ref="BL37:BL38"/>
+    <mergeCell ref="BM37:BM38"/>
+    <mergeCell ref="BN37:BN38"/>
+    <mergeCell ref="BE37:BE38"/>
+    <mergeCell ref="BF37:BF38"/>
+    <mergeCell ref="BG37:BG38"/>
+    <mergeCell ref="BH37:BH38"/>
+    <mergeCell ref="BI37:BI38"/>
+    <mergeCell ref="AZ37:AZ38"/>
+    <mergeCell ref="BA37:BA38"/>
+    <mergeCell ref="BB37:BB38"/>
+    <mergeCell ref="BC37:BC38"/>
+    <mergeCell ref="BD37:BD38"/>
+    <mergeCell ref="AU37:AU38"/>
+    <mergeCell ref="AV37:AV38"/>
+    <mergeCell ref="AW37:AW38"/>
+    <mergeCell ref="AX37:AX38"/>
+    <mergeCell ref="AY37:AY38"/>
+    <mergeCell ref="AP37:AP38"/>
+    <mergeCell ref="AQ37:AQ38"/>
+    <mergeCell ref="AR37:AR38"/>
+    <mergeCell ref="AS37:AS38"/>
+    <mergeCell ref="AT37:AT38"/>
+    <mergeCell ref="AK37:AK38"/>
+    <mergeCell ref="AL37:AL38"/>
+    <mergeCell ref="AM37:AM38"/>
+    <mergeCell ref="AN37:AN38"/>
+    <mergeCell ref="AO37:AO38"/>
+    <mergeCell ref="AF37:AF38"/>
+    <mergeCell ref="AG37:AG38"/>
+    <mergeCell ref="AH37:AH38"/>
+    <mergeCell ref="AI37:AI38"/>
+    <mergeCell ref="AJ37:AJ38"/>
+    <mergeCell ref="AA37:AA38"/>
+    <mergeCell ref="AB37:AB38"/>
+    <mergeCell ref="AC37:AC38"/>
+    <mergeCell ref="AD37:AD38"/>
+    <mergeCell ref="AE37:AE38"/>
+    <mergeCell ref="V37:V38"/>
+    <mergeCell ref="W37:W38"/>
+    <mergeCell ref="X37:X38"/>
+    <mergeCell ref="Y37:Y38"/>
+    <mergeCell ref="Z37:Z38"/>
+    <mergeCell ref="Q37:Q38"/>
+    <mergeCell ref="R37:R38"/>
+    <mergeCell ref="S37:S38"/>
+    <mergeCell ref="T37:T38"/>
+    <mergeCell ref="U37:U38"/>
+    <mergeCell ref="L37:L38"/>
+    <mergeCell ref="M37:M38"/>
+    <mergeCell ref="N37:N38"/>
+    <mergeCell ref="O37:O38"/>
+    <mergeCell ref="P37:P38"/>
+    <mergeCell ref="G37:G38"/>
+    <mergeCell ref="H37:H38"/>
+    <mergeCell ref="I37:I38"/>
+    <mergeCell ref="J37:J38"/>
+    <mergeCell ref="K37:K38"/>
+    <mergeCell ref="A35:F35"/>
+    <mergeCell ref="A37:A38"/>
+    <mergeCell ref="B37:B38"/>
+    <mergeCell ref="C37:C38"/>
+    <mergeCell ref="D37:D38"/>
+    <mergeCell ref="E37:E38"/>
+    <mergeCell ref="F37:F38"/>
+    <mergeCell ref="A25:D25"/>
+    <mergeCell ref="A27:D27"/>
+    <mergeCell ref="A29:F29"/>
+    <mergeCell ref="A31:F31"/>
+    <mergeCell ref="A33:J33"/>
+    <mergeCell ref="A15:D15"/>
+    <mergeCell ref="A17:D17"/>
+    <mergeCell ref="A19:E19"/>
+    <mergeCell ref="A21:J21"/>
+    <mergeCell ref="A23:F23"/>
+    <mergeCell ref="A5:E5"/>
+    <mergeCell ref="A7:F7"/>
+    <mergeCell ref="A9:F9"/>
+    <mergeCell ref="A11:F11"/>
+    <mergeCell ref="A13:E13"/>
     <mergeCell ref="DG2:DR2"/>
     <mergeCell ref="DS2:ED2"/>
     <mergeCell ref="EE2:EP2"/>
@@ -19595,90 +19679,6 @@
     <mergeCell ref="BQ2:CB2"/>
     <mergeCell ref="CC2:CR2"/>
     <mergeCell ref="CS2:DF2"/>
-    <mergeCell ref="A5:E5"/>
-    <mergeCell ref="A7:F7"/>
-    <mergeCell ref="A9:F9"/>
-    <mergeCell ref="A11:F11"/>
-    <mergeCell ref="A13:E13"/>
-    <mergeCell ref="A15:D15"/>
-    <mergeCell ref="A17:D17"/>
-    <mergeCell ref="A19:E19"/>
-    <mergeCell ref="A21:J21"/>
-    <mergeCell ref="A23:F23"/>
-    <mergeCell ref="A25:D25"/>
-    <mergeCell ref="A27:D27"/>
-    <mergeCell ref="A29:F29"/>
-    <mergeCell ref="A31:F31"/>
-    <mergeCell ref="A33:J33"/>
-    <mergeCell ref="A35:F35"/>
-    <mergeCell ref="A37:A38"/>
-    <mergeCell ref="B37:B38"/>
-    <mergeCell ref="C37:C38"/>
-    <mergeCell ref="D37:D38"/>
-    <mergeCell ref="E37:E38"/>
-    <mergeCell ref="F37:F38"/>
-    <mergeCell ref="G37:G38"/>
-    <mergeCell ref="H37:H38"/>
-    <mergeCell ref="I37:I38"/>
-    <mergeCell ref="J37:J38"/>
-    <mergeCell ref="K37:K38"/>
-    <mergeCell ref="L37:L38"/>
-    <mergeCell ref="M37:M38"/>
-    <mergeCell ref="N37:N38"/>
-    <mergeCell ref="O37:O38"/>
-    <mergeCell ref="P37:P38"/>
-    <mergeCell ref="Q37:Q38"/>
-    <mergeCell ref="R37:R38"/>
-    <mergeCell ref="S37:S38"/>
-    <mergeCell ref="T37:T38"/>
-    <mergeCell ref="U37:U38"/>
-    <mergeCell ref="V37:V38"/>
-    <mergeCell ref="W37:W38"/>
-    <mergeCell ref="X37:X38"/>
-    <mergeCell ref="Y37:Y38"/>
-    <mergeCell ref="Z37:Z38"/>
-    <mergeCell ref="AA37:AA38"/>
-    <mergeCell ref="AB37:AB38"/>
-    <mergeCell ref="AC37:AC38"/>
-    <mergeCell ref="AD37:AD38"/>
-    <mergeCell ref="AE37:AE38"/>
-    <mergeCell ref="AF37:AF38"/>
-    <mergeCell ref="AG37:AG38"/>
-    <mergeCell ref="AH37:AH38"/>
-    <mergeCell ref="AI37:AI38"/>
-    <mergeCell ref="AJ37:AJ38"/>
-    <mergeCell ref="AK37:AK38"/>
-    <mergeCell ref="AL37:AL38"/>
-    <mergeCell ref="AM37:AM38"/>
-    <mergeCell ref="AN37:AN38"/>
-    <mergeCell ref="AO37:AO38"/>
-    <mergeCell ref="AP37:AP38"/>
-    <mergeCell ref="AQ37:AQ38"/>
-    <mergeCell ref="AR37:AR38"/>
-    <mergeCell ref="AS37:AS38"/>
-    <mergeCell ref="AT37:AT38"/>
-    <mergeCell ref="AU37:AU38"/>
-    <mergeCell ref="AV37:AV38"/>
-    <mergeCell ref="AW37:AW38"/>
-    <mergeCell ref="AX37:AX38"/>
-    <mergeCell ref="AY37:AY38"/>
-    <mergeCell ref="AZ37:AZ38"/>
-    <mergeCell ref="BA37:BA38"/>
-    <mergeCell ref="BB37:BB38"/>
-    <mergeCell ref="BC37:BC38"/>
-    <mergeCell ref="BD37:BD38"/>
-    <mergeCell ref="BE37:BE38"/>
-    <mergeCell ref="BF37:BF38"/>
-    <mergeCell ref="BG37:BG38"/>
-    <mergeCell ref="BH37:BH38"/>
-    <mergeCell ref="BI37:BI38"/>
-    <mergeCell ref="BO37:BO38"/>
-    <mergeCell ref="BP37:BP38"/>
-    <mergeCell ref="BJ37:BJ38"/>
-    <mergeCell ref="BK37:BK38"/>
-    <mergeCell ref="BL37:BL38"/>
-    <mergeCell ref="BM37:BM38"/>
-    <mergeCell ref="BN37:BN38"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait"/>
@@ -24106,8 +24106,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C886C271-C803-433F-9D5E-7E0C5EDF0D99}">
   <dimension ref="A1:T162"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="72" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView tabSelected="1" topLeftCell="A72" zoomScale="72" workbookViewId="0">
+      <selection activeCell="T94" sqref="T94"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" customHeight="1"/>

</xml_diff>